<commit_message>
add html pages (version1.1)
</commit_message>
<xml_diff>
--- a/SchemaInfo.xlsx
+++ b/SchemaInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yudai\OneDrive - 筑波大学\prog\LOD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yudai\OneDrive - 筑波大学\prog\LOD\tvstation-lod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3C9C46D-8FAD-4BA5-A6D5-B440AE7D6D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297AAC9C-1FFA-4854-999D-F92900733098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="876" windowWidth="12972" windowHeight="12084" xr2:uid="{FBBF9BC9-1442-45DB-A650-E7CA57B7D212}"/>
+    <workbookView xWindow="1248" yWindow="564" windowWidth="12972" windowHeight="12084" xr2:uid="{FBBF9BC9-1442-45DB-A650-E7CA57B7D212}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="178">
   <si>
     <t>電波種類</t>
     <rPh sb="0" eb="4">
@@ -955,33 +955,21 @@
     <t>https://www.wikidata.org/prop/direct/P3225</t>
   </si>
   <si>
-    <t>schema:ownershipFundingInfo</t>
-  </si>
-  <si>
     <t>https://schema.org/ownershipFundingInfo</t>
   </si>
   <si>
     <t>事業者URI</t>
   </si>
   <si>
-    <t>schema:parentOrganization</t>
-  </si>
-  <si>
     <t>https://schema.org/parentOrganization</t>
   </si>
   <si>
     <t>ブロック</t>
   </si>
   <si>
-    <t>tvst:networkBlock</t>
-  </si>
-  <si>
     <t>https://w3id.org/tvstationjp/tvst/networkBlock</t>
   </si>
   <si>
-    <t>schema:brand</t>
-  </si>
-  <si>
     <t>https://schema.org/brand</t>
   </si>
   <si>
@@ -1075,9 +1063,6 @@
     <t>https://w3id.org/tvstationjp/tvst/callName</t>
   </si>
   <si>
-    <t>tvst:beginningDate</t>
-  </si>
-  <si>
     <t>https://w3id.org/tvstationjp/tvst/beginningDate</t>
   </si>
   <si>
@@ -1087,9 +1072,6 @@
     <t>https://w3id.org/tvstationjp/platform</t>
   </si>
   <si>
-    <t>tvst:chPosition</t>
-  </si>
-  <si>
     <t>https://w3id.org/tvstationjp/tvst/chPosition</t>
   </si>
   <si>
@@ -1100,9 +1082,6 @@
   </si>
   <si>
     <t>https://w3id.org/tvstationjp/tvst/parentStation</t>
-  </si>
-  <si>
-    <t>tvst:parentDTVCh</t>
   </si>
   <si>
     <t>https://w3id.org/tvstationjp/tvst/parentDTVCh</t>
@@ -1145,6 +1124,42 @@
     <rPh sb="12" eb="14">
       <t>セイスウ</t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>schema:ownershipFundingInfo</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>schema:parentOrganization</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>tvst:networkBlock</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>schema:brand</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>schema:address</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>schema:longitude</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>tvst:beginningDate</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>tvst:chPosition</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>tvst:parentDTVCh</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1551,7 +1566,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D214439-3BEB-4354-A594-4BF144B8F407}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1573,7 +1590,7 @@
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>74</v>
@@ -1720,7 +1737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="54" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -2121,16 +2138,16 @@
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>103</v>
@@ -2141,16 +2158,16 @@
         <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>103</v>
@@ -2158,13 +2175,13 @@
     </row>
     <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>122</v>
+        <v>171</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>33</v>
@@ -2181,16 +2198,16 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>94</v>
@@ -2201,16 +2218,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>127</v>
+        <v>173</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>103</v>
@@ -2221,10 +2238,10 @@
         <v>38</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>39</v>
@@ -2241,16 +2258,16 @@
         <v>40</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>103</v>
@@ -2261,16 +2278,16 @@
         <v>42</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>135</v>
+        <v>174</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>103</v>
@@ -2281,13 +2298,13 @@
         <v>44</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>77</v>
@@ -2298,16 +2315,16 @@
     </row>
     <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>77</v>
@@ -2318,16 +2335,16 @@
     </row>
     <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>77</v>
@@ -2345,7 +2362,7 @@
     </row>
     <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>45</v>
@@ -2439,10 +2456,10 @@
         <v>47</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>48</v>
@@ -2459,10 +2476,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>51</v>
@@ -2479,10 +2496,10 @@
         <v>53</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>54</v>
@@ -2519,13 +2536,13 @@
         <v>55</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>110</v>
@@ -2539,10 +2556,10 @@
         <v>56</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>57</v>
@@ -2559,10 +2576,10 @@
         <v>58</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>59</v>
@@ -2599,16 +2616,16 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>60</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="F58" s="7"/>
     </row>
@@ -2617,16 +2634,16 @@
         <v>61</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>103</v>
@@ -2634,13 +2651,13 @@
     </row>
     <row r="60" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>63</v>
@@ -2657,10 +2674,10 @@
         <v>64</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>65</v>
@@ -2674,13 +2691,13 @@
     </row>
     <row r="62" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>66</v>
@@ -2697,16 +2714,16 @@
         <v>67</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>94</v>
@@ -2717,16 +2734,16 @@
         <v>36</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>103</v>
@@ -2737,10 +2754,10 @@
         <v>69</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>70</v>
@@ -2757,16 +2774,16 @@
         <v>40</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>103</v>
@@ -2777,16 +2794,16 @@
         <v>42</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>103</v>
@@ -2797,13 +2814,13 @@
         <v>44</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>77</v>
@@ -2814,16 +2831,16 @@
     </row>
     <row r="69" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>77</v>
@@ -2834,16 +2851,16 @@
     </row>
     <row r="70" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>77</v>
@@ -2855,5 +2872,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>